<commit_message>
added data parameters for excel
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,55 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>A234wd</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>TCID</t>
   </si>
@@ -77,22 +33,25 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>runmode</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>george2c@optusnet.com.au</t>
+  </si>
+  <si>
+    <t>Selenium@123</t>
   </si>
 </sst>
 </file>
@@ -402,7 +361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,34 +382,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -460,128 +403,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added second testcase for POM
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
+    <sheet name="CreateAccountTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -52,6 +53,15 @@
   </si>
   <si>
     <t>Selenium@123</t>
+  </si>
+  <si>
+    <t>CreateAccountTest</t>
+  </si>
+  <si>
+    <t>accountname</t>
+  </si>
+  <si>
+    <t>george</t>
   </si>
 </sst>
 </file>
@@ -369,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,6 +403,14 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -440,4 +458,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>